<commit_message>
update hrms and voc
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/public/wwwroot/templates/ShifTemplate.xlsx
+++ b/ASP.NET CORE/HRMNS/public/wwwroot/templates/ShifTemplate.xlsx
@@ -23,12 +23,6 @@
     <t>Ca Lam Viec</t>
   </si>
   <si>
-    <t>Ngay Bat Dau</t>
-  </si>
-  <si>
-    <t>Ngay Ket Thuc</t>
-  </si>
-  <si>
     <t>CD_WHC</t>
   </si>
   <si>
@@ -42,6 +36,12 @@
   </si>
   <si>
     <t>H2105001</t>
+  </si>
+  <si>
+    <t>Tên NV</t>
+  </si>
+  <si>
+    <t>XXXX</t>
   </si>
 </sst>
 </file>
@@ -104,12 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,44 +416,38 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="1" max="3" width="24.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="4">
-        <v>44197</v>
-      </c>
-      <c r="D2" s="4">
-        <v>44211</v>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -466,7 +459,7 @@
           <x14:formula1>
             <xm:f>'DM CaLviec'!$B$1:$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>B1 B2</xm:sqref>
+          <xm:sqref>C1 C2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -494,18 +487,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>